<commit_message>
Zrobiona struktura krzyżówki, trzeba poprawić wymiary i responsywność
</commit_message>
<xml_diff>
--- a/KRZYZOWKA.xlsx
+++ b/KRZYZOWKA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KONRAD\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KONRAD\Desktop\witryny projekt termin do 11 października\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="25">
   <si>
     <t>I</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>13 wysokosc</t>
+  </si>
+  <si>
+    <t>14 szerokosc</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -202,6 +214,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -482,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +509,7 @@
     <col min="17" max="17" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,344 +544,400 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E7">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="G7">
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
         <v>5</v>
       </c>
-      <c r="J7">
-        <v>6</v>
-      </c>
-      <c r="K7">
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
         <v>7</v>
       </c>
-      <c r="L7">
+      <c r="K6">
         <v>8</v>
       </c>
-      <c r="M7">
+      <c r="L6">
         <v>9</v>
       </c>
-      <c r="N7">
+      <c r="M6">
         <v>10</v>
       </c>
-      <c r="O7">
+      <c r="N6">
         <v>11</v>
       </c>
-      <c r="P7">
+      <c r="O6">
         <v>12</v>
       </c>
-      <c r="Q7">
+      <c r="P6">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D8">
+      <c r="Q6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D7" s="12">
         <v>1</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D8" s="12">
+        <v>2</v>
+      </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D9">
+      <c r="O8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="13"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D9" s="12">
+        <v>3</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>2</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="13"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D10" s="12">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="13"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D11" s="12">
         <v>5</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <v>4</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="R11" s="13"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D12" s="12">
+        <v>6</v>
+      </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="7" t="s">
+      <c r="J12" s="2"/>
+      <c r="O12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R12" s="13"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D13" s="12">
         <v>7</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D13">
-        <v>6</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="O13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D14">
+      <c r="Q13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R13" s="13"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D14" s="12">
+        <v>8</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J14" s="2"/>
+      <c r="L14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="Q14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" s="13"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D15" s="12">
+        <v>9</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="13"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D16" s="12">
+        <v>10</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R16" s="13"/>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D17" s="12">
+        <v>11</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D15">
+      <c r="Q17" s="12"/>
+      <c r="R17" s="13"/>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D18" s="12">
+        <v>12</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="13"/>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D16">
+      <c r="N22" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="K17" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <v>11</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D19">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" t="s">
-        <v>5</v>
-      </c>
-      <c r="K23" t="s">
-        <v>6</v>
-      </c>
-      <c r="L23" t="s">
-        <v>7</v>
-      </c>
-      <c r="M23" t="s">
-        <v>8</v>
-      </c>
-      <c r="N23" t="s">
-        <v>9</v>
-      </c>
-      <c r="O23" t="s">
+      <c r="O22" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>